<commit_message>
Update nutrient component calculation
</commit_message>
<xml_diff>
--- a/Create Database.xlsx
+++ b/Create Database.xlsx
@@ -8,32 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\private\Practice_code\hackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18EC131E-024C-409E-B616-CC11A7BF9559}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FAF769-2306-454C-9AA0-84321B2D1013}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="3165" windowWidth="21600" windowHeight="11385" xr2:uid="{BAAD5386-AA5D-4A59-9F86-234F07EB8587}"/>
+    <workbookView xWindow="3630" yWindow="3720" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>code</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -68,6 +60,50 @@
   </si>
   <si>
     <t>똑볶이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>provision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kcal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carbo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sugar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>protein</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sat_fat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tra_fat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colestrol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>natrium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -100,12 +136,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -114,9 +165,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -431,80 +488,173 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0EEAAD-1A90-46CD-A2C8-8508A8FA8A5D}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.625" customWidth="1"/>
-    <col min="3" max="3" width="29.375" customWidth="1"/>
+    <col min="1" max="17" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>8801062521906</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1400</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1">
+        <v>100</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1">
+        <v>245</v>
+      </c>
+      <c r="J2" s="1">
+        <v>33</v>
+      </c>
+      <c r="K2" s="2">
+        <v>4</v>
+      </c>
+      <c r="L2" s="2">
+        <v>3</v>
+      </c>
+      <c r="M2" s="2">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2">
+        <v>6</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0.4</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>8801117752804</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>2400</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>8801019604034</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>1100</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Update images and DB
</commit_message>
<xml_diff>
--- a/Create Database.xlsx
+++ b/Create Database.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\private\Practice_code\hackathon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이재윤\Desktop\lasthack-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C4DC5A-59DC-4912-B287-CCCDCB098B54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9108"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>code</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,18 +50,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>과자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오감자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>똑볶이</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>provision</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -128,13 +115,45 @@
   </si>
   <si>
     <t>오리온</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>롯데</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에어베이크드 포테이토</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>꼬깔콘(군옥수수맛)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빼빼로(오리지널맛)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빼빼로(쿠키앤크림맛)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>초코파이(12봉)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엄마손파이(10봉)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>칙촉</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -189,7 +208,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -197,6 +216,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -512,19 +534,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="18" width="12.75" customWidth="1"/>
+    <col min="1" max="1" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="19" width="12.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -538,43 +567,43 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>3</v>
@@ -583,230 +612,522 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>8801062521906</v>
+        <v>8801043036672</v>
       </c>
       <c r="C2" s="1">
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="F2" s="1">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1">
+        <v>30</v>
+      </c>
+      <c r="I2" s="1">
+        <v>150</v>
+      </c>
+      <c r="J2" s="1">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
         <v>2</v>
       </c>
-      <c r="H2" s="1">
-        <v>50</v>
-      </c>
-      <c r="I2" s="1">
-        <v>245</v>
-      </c>
-      <c r="J2" s="1">
-        <v>33</v>
-      </c>
-      <c r="K2" s="2">
-        <v>4</v>
-      </c>
-      <c r="L2" s="2">
-        <v>3</v>
-      </c>
       <c r="M2" s="2">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="N2" s="2">
-        <v>6</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="O2" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P2" s="2">
         <v>0</v>
       </c>
       <c r="Q2" s="2">
-        <v>0.4</v>
+        <v>220</v>
       </c>
       <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
+      <c r="S2" s="3">
+        <v>44116</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>8801117752804</v>
+        <v>8801117747602</v>
       </c>
       <c r="C3" s="1">
-        <v>2400</v>
+        <v>1500</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1">
+        <v>155</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1">
+        <v>30</v>
+      </c>
+      <c r="I3" s="1">
+        <v>156</v>
+      </c>
+      <c r="J3" s="1">
+        <v>18</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>3</v>
+      </c>
+      <c r="M3" s="1">
+        <v>8</v>
+      </c>
+      <c r="N3" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>190</v>
+      </c>
       <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
+      <c r="S3" s="3">
+        <v>44116</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>8801019604034</v>
+        <v>8801062880331</v>
       </c>
       <c r="C4" s="1">
-        <v>1100</v>
+        <v>1800</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1">
+        <v>130</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>30</v>
+      </c>
+      <c r="I4" s="1">
+        <v>130</v>
+      </c>
+      <c r="J4" s="1">
+        <v>23</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>3</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>180</v>
+      </c>
       <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
+      <c r="S4" s="3">
+        <v>44116</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>8801043036672</v>
+        <v>8801062380213</v>
       </c>
       <c r="C5" s="1">
-        <v>1200</v>
+        <v>1500</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G5" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H5" s="1">
         <v>30</v>
       </c>
       <c r="I5" s="1">
-        <v>150</v>
+        <v>205</v>
       </c>
       <c r="J5" s="1">
-        <v>20</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2">
+        <v>21</v>
+      </c>
+      <c r="K5" s="1">
         <v>2</v>
       </c>
-      <c r="M5" s="2">
-        <v>7</v>
-      </c>
-      <c r="N5" s="2">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="O5" s="2">
-        <v>0</v>
-      </c>
-      <c r="P5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0.22</v>
+      <c r="L5" s="1">
+        <v>2</v>
+      </c>
+      <c r="M5" s="1">
+        <v>12</v>
+      </c>
+      <c r="N5" s="1">
+        <v>4</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>155</v>
       </c>
       <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
+      <c r="S5" s="3">
+        <v>44116</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>8801117747602</v>
+        <v>8801062012701</v>
       </c>
       <c r="C6" s="1">
-        <v>3500</v>
+        <v>1200</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1">
-        <v>155</v>
+        <v>54</v>
       </c>
       <c r="G6" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H6" s="1">
         <v>30</v>
       </c>
       <c r="I6" s="1">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="J6" s="1">
         <v>18</v>
       </c>
       <c r="K6" s="1">
+        <v>7</v>
+      </c>
+      <c r="L6" s="1">
+        <v>2</v>
+      </c>
+      <c r="M6" s="1">
+        <v>6</v>
+      </c>
+      <c r="N6" s="1">
+        <v>3</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>125</v>
+      </c>
+      <c r="R6" s="1"/>
+      <c r="S6" s="3">
+        <v>44116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>8801062012732</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1200</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1">
+        <v>37</v>
+      </c>
+      <c r="G7" s="1">
         <v>1</v>
       </c>
-      <c r="L6" s="1">
+      <c r="H7" s="1">
+        <v>30</v>
+      </c>
+      <c r="I7" s="1">
+        <v>190</v>
+      </c>
+      <c r="J7" s="1">
+        <v>26</v>
+      </c>
+      <c r="K7" s="1">
+        <v>14</v>
+      </c>
+      <c r="L7" s="1">
         <v>3</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M7" s="1">
         <v>8</v>
       </c>
-      <c r="N6" s="1">
-        <v>3.6</v>
-      </c>
-      <c r="O6" s="1">
+      <c r="N7" s="1">
+        <v>8</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>140</v>
+      </c>
+      <c r="R7" s="1"/>
+      <c r="S7" s="3">
+        <v>44116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8801062894659</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3600</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1">
+        <v>336</v>
+      </c>
+      <c r="G8" s="1">
+        <v>12</v>
+      </c>
+      <c r="H8" s="1">
+        <v>30</v>
+      </c>
+      <c r="I8" s="1">
+        <v>120</v>
+      </c>
+      <c r="J8" s="1">
+        <v>18</v>
+      </c>
+      <c r="K8" s="1">
+        <v>10</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1">
+        <v>4</v>
+      </c>
+      <c r="N8" s="1">
+        <v>3</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>65</v>
+      </c>
+      <c r="R8" s="1"/>
+      <c r="S8" s="3">
+        <v>44116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8801062521241</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2800</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="1">
+        <v>127</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>100</v>
+      </c>
+      <c r="I9" s="1">
+        <v>500</v>
+      </c>
+      <c r="J9" s="1">
+        <v>57</v>
+      </c>
+      <c r="K9" s="1">
         <v>0.1</v>
       </c>
-      <c r="P6" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>0.19</v>
-      </c>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
+      <c r="L9" s="1">
+        <v>8</v>
+      </c>
+      <c r="M9" s="1">
+        <v>24</v>
+      </c>
+      <c r="N9" s="1">
+        <v>13</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>370</v>
+      </c>
+      <c r="R9" s="1"/>
+      <c r="S9" s="3">
+        <v>44116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>8801062247431</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3200</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="1">
+        <v>90</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>90</v>
+      </c>
+      <c r="I10" s="1">
+        <v>440</v>
+      </c>
+      <c r="J10" s="1">
+        <v>54</v>
+      </c>
+      <c r="K10" s="1">
+        <v>30</v>
+      </c>
+      <c r="L10" s="1">
+        <v>6</v>
+      </c>
+      <c r="M10" s="1">
+        <v>22</v>
+      </c>
+      <c r="N10" s="1">
+        <v>15</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>290</v>
+      </c>
+      <c r="R10" s="1"/>
+      <c r="S10" s="3">
+        <v>44116</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>